<commit_message>
Primary Member Details screen TC added
</commit_message>
<xml_diff>
--- a/BESTDDFinalVersion2/src/test/java/testdata/TestData.xlsx
+++ b/BESTDDFinalVersion2/src/test/java/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BEA65F-3FB1-4ACE-9AD8-B47BEB84AF73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4185D6DD-85AF-4B8D-A2AF-EC1D3D3B3EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="0" windowWidth="20244" windowHeight="12360" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchforPlan" sheetId="3" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <sheet name="CreateCustomer" sheetId="10" r:id="rId7"/>
     <sheet name="AddCC" sheetId="8" r:id="rId8"/>
     <sheet name="AddPM" sheetId="11" r:id="rId9"/>
+    <sheet name="AddPrimaryMember" sheetId="12" r:id="rId10"/>
+    <sheet name="AddDependent" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="170">
   <si>
     <t>don1thack</t>
   </si>
@@ -445,13 +447,106 @@
   </si>
   <si>
     <t>Always Print and Mail</t>
+  </si>
+  <si>
+    <t>Cust_Num</t>
+  </si>
+  <si>
+    <t>53569687</t>
+  </si>
+  <si>
+    <t>Maritalstatus</t>
+  </si>
+  <si>
+    <t>P_Address</t>
+  </si>
+  <si>
+    <t>18 test street</t>
+  </si>
+  <si>
+    <t>emailaddress</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>ashraf</t>
+  </si>
+  <si>
+    <t>t_7ryr@test.com</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>soha</t>
+  </si>
+  <si>
+    <t>PrimaryNum</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Eligible</t>
+  </si>
+  <si>
+    <t>Eligible Reason</t>
+  </si>
+  <si>
+    <t>ProofDate</t>
+  </si>
+  <si>
+    <t>DependentTest1</t>
+  </si>
+  <si>
+    <t>Testyo</t>
+  </si>
+  <si>
+    <t>child</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>Disability</t>
+  </si>
+  <si>
+    <t>DependentTest2</t>
+  </si>
+  <si>
+    <t>Under Age</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>DependentTest3</t>
+  </si>
+  <si>
+    <t>spouse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,6 +568,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -482,7 +583,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -525,11 +626,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -554,11 +692,327 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -569,6 +1023,48 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{34B0327B-A0B8-4111-AA20-E424D4A45775}" name="Table2" displayName="Table2" ref="A1:L2" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+  <autoFilter ref="A1:L2" xr:uid="{34B0327B-A0B8-4111-AA20-E424D4A45775}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{F4E4B232-FF71-46A3-A968-CD5074D2B476}" name="UserName" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{F2D0DEBC-843E-4988-A083-D2B2880184EC}" name="Password" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{A6DF7E19-7AAE-4FB1-9D1E-96ABD3A4626C}" name="Cust_Num" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{2BD52C4C-CB4B-453B-A505-0EC08C15FE0E}" name="Firstname" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{B1746E98-760D-4020-A3CD-FCCC7F23B355}" name="Lastname" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{C978D836-5D84-4723-AFC4-93804C6ACAEB}" name="emailaddress" dataDxfId="6" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{1A7888B2-FE0B-4B91-8762-E09D17DC1696}" name="P_Address" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{A0A4E9E7-B5BB-4C81-863E-760D1B9B174F}" name="ZiPCode" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{F7F31B1B-DE17-49F5-9BD8-139153CD882C}" name="Agee" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{992B2615-7D38-4198-B472-3FD7201DBD14}" name="Gender" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{96EBDB42-7126-43BF-8316-78F7A6076B35}" name="Maritalstatus" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{ED65F2A4-EC55-42CB-9102-9DB306AA44E4}" name="SSN" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F32D3563-CFEB-4FA8-B27D-602AE7D03C08}" name="Table1" displayName="Table1" ref="A1:L5" totalsRowShown="0">
+  <autoFilter ref="A1:L5" xr:uid="{F32D3563-CFEB-4FA8-B27D-602AE7D03C08}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{C99AF76A-24F6-4F24-AF9D-10DA3DD5FC79}" name="UserName"/>
+    <tableColumn id="2" xr3:uid="{6BF3CD8D-763D-493A-A001-844C1E92F61B}" name="Password"/>
+    <tableColumn id="3" xr3:uid="{74969F41-58A1-42F5-87DB-FD6C56419485}" name="CustomerNum"/>
+    <tableColumn id="4" xr3:uid="{3A2C8D80-7C90-40D9-978A-779336809B9E}" name="PrimaryNum"/>
+    <tableColumn id="5" xr3:uid="{0FA27347-788D-4FF9-BD7C-7F1050C376DA}" name="FirstName"/>
+    <tableColumn id="6" xr3:uid="{D29F01E7-1F8A-4024-9BCD-0B4B61C6B837}" name="LastName"/>
+    <tableColumn id="7" xr3:uid="{58D22FA4-E7F0-4B3D-B2EC-F3FEFF5F23F9}" name="Relationship"/>
+    <tableColumn id="8" xr3:uid="{8DA309DA-030E-44BE-8DE3-D1AFB282AC18}" name="Age"/>
+    <tableColumn id="9" xr3:uid="{E87A0500-8328-4687-B6D1-7B12B8A41677}" name="Gender"/>
+    <tableColumn id="10" xr3:uid="{793D875A-E782-4370-B142-8423CAC00DB5}" name="Eligible"/>
+    <tableColumn id="11" xr3:uid="{A425EE86-9D51-4176-B0D9-287AC8F5BDEA}" name="Eligible Reason"/>
+    <tableColumn id="12" xr3:uid="{8E382D37-DB05-4569-95D8-5773D948E021}" name="ProofDate"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -895,6 +1391,333 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530E5594-3326-40BB-9DE0-ED5268032DC2}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" customWidth="1"/>
+    <col min="12" max="12" width="10" style="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="15">
+        <v>75202</v>
+      </c>
+      <c r="I2" s="15">
+        <v>25</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F33BEB1-5052-4610-AA2F-CD787A268AAB}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>53570720</v>
+      </c>
+      <c r="D2">
+        <v>105698752</v>
+      </c>
+      <c r="E2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" t="s">
+        <v>164</v>
+      </c>
+      <c r="L2" s="24">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>53570720</v>
+      </c>
+      <c r="D3">
+        <v>105698752</v>
+      </c>
+      <c r="E3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G3" t="s">
+        <v>162</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>149</v>
+      </c>
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" t="s">
+        <v>166</v>
+      </c>
+      <c r="L3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>53570720</v>
+      </c>
+      <c r="D4">
+        <v>105698752</v>
+      </c>
+      <c r="E4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>163</v>
+      </c>
+      <c r="J4" t="s">
+        <v>167</v>
+      </c>
+      <c r="K4" t="s">
+        <v>167</v>
+      </c>
+      <c r="L4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>53570720</v>
+      </c>
+      <c r="D5">
+        <v>105698752</v>
+      </c>
+      <c r="E5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G5" t="s">
+        <v>162</v>
+      </c>
+      <c r="H5">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>163</v>
+      </c>
+      <c r="J5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0115254B-3FE7-4242-96FF-AEEA810EA1D4}">
   <dimension ref="A1:G7"/>
@@ -1085,7 +1908,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1839,8 +2662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD6177A-7BF6-452C-B399-7E27930614E1}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adding updated testdata file amd missing change in PrimaryMembersscreen
</commit_message>
<xml_diff>
--- a/BESTDDFinalVersion2/src/test/java/testdata/TestData.xlsx
+++ b/BESTDDFinalVersion2/src/test/java/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD90270B-5384-492C-A061-3B5F982730AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426A4382-D323-4466-8655-9CE1EA476348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchforPlan" sheetId="3" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="AddDependentCase" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="174">
   <si>
     <t>don1thack</t>
   </si>
@@ -522,6 +523,36 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>Dental</t>
+  </si>
+  <si>
+    <t>EffectiveDate</t>
+  </si>
+  <si>
+    <t>01/01/2022</t>
+  </si>
+  <si>
+    <t>01/01/2023</t>
+  </si>
+  <si>
+    <t>EnrollmentReason</t>
+  </si>
+  <si>
+    <t>Initial Enrollment</t>
+  </si>
+  <si>
+    <t>MajorEffectiveDate</t>
+  </si>
+  <si>
+    <t>WaitingPeriod</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -559,7 +590,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -602,11 +633,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -636,6 +678,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -982,7 +1025,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD5"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1193,15 +1236,22 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9FEB4D-EC75-4F1A-9E57-6A856A099F59}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:L1048576"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1214,8 +1264,23 @@
       <c r="D1" s="12" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1228,9 +1293,25 @@
       <c r="D2" s="13" t="s">
         <v>154</v>
       </c>
+      <c r="E2" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>170</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
AddDependentAndCase test and refining AddDependentCase test
</commit_message>
<xml_diff>
--- a/BESTDDFinalVersion2/src/test/java/testdata/TestData.xlsx
+++ b/BESTDDFinalVersion2/src/test/java/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426A4382-D323-4466-8655-9CE1EA476348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A941960F-85B5-421D-B04D-91BFDD8E8EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchforPlan" sheetId="3" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="AddPM" sheetId="11" r:id="rId9"/>
     <sheet name="AddDependent" sheetId="12" r:id="rId10"/>
     <sheet name="AddDependentCase" sheetId="13" r:id="rId11"/>
+    <sheet name="AddDependentAndCase" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="180">
   <si>
     <t>don1thack</t>
   </si>
@@ -553,6 +553,24 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>DependentFName</t>
+  </si>
+  <si>
+    <t>105729197</t>
+  </si>
+  <si>
+    <t>Dep Fname</t>
+  </si>
+  <si>
+    <t>DependentTestC1</t>
+  </si>
+  <si>
+    <t>DependentTestC2</t>
+  </si>
+  <si>
+    <t>Testlname</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1043,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1236,22 +1254,23 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9FEB4D-EC75-4F1A-9E57-6A856A099F59}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1264,23 +1283,26 @@
       <c r="D1" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1291,27 +1313,212 @@
         <v>140</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>170</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43B5AB1-17D0-4ED9-B394-C04ADAA702DB}">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Primary member Details Page splitted from Life Primary Member Details screen
</commit_message>
<xml_diff>
--- a/BESTDDFinalVersion2/src/test/java/testdata/TestData.xlsx
+++ b/BESTDDFinalVersion2/src/test/java/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426A4382-D323-4466-8655-9CE1EA476348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E61B02A-C643-4138-8799-1C1FFA6CF01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="0" windowWidth="20244" windowHeight="12360" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchforPlan" sheetId="3" r:id="rId1"/>
@@ -17,21 +17,31 @@
     <sheet name="CreateCustomer" sheetId="10" r:id="rId7"/>
     <sheet name="AddCC" sheetId="8" r:id="rId8"/>
     <sheet name="AddPM" sheetId="11" r:id="rId9"/>
-    <sheet name="AddDependent" sheetId="12" r:id="rId10"/>
-    <sheet name="AddDependentCase" sheetId="13" r:id="rId11"/>
+    <sheet name="AddPrimaryMember" sheetId="14" r:id="rId10"/>
+    <sheet name="AddDependent" sheetId="12" r:id="rId11"/>
+    <sheet name="AddDependentCase" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="184">
   <si>
     <t>don1thack</t>
   </si>
@@ -553,6 +563,36 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>t_7ryr@test.com</t>
+  </si>
+  <si>
+    <t>18 test street</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>emailaddress</t>
+  </si>
+  <si>
+    <t>P_Address</t>
+  </si>
+  <si>
+    <t>Maritalstatus</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>akram</t>
+  </si>
+  <si>
+    <t>53583894</t>
+  </si>
+  <si>
+    <t>tina</t>
   </si>
 </sst>
 </file>
@@ -648,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -679,6 +719,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,6 +1064,100 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9302E6BE-0119-4799-BFCE-37A6D7C55B45}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.5546875" style="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2">
+        <v>75202</v>
+      </c>
+      <c r="I2">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>146</v>
+      </c>
+      <c r="K2" t="s">
+        <v>176</v>
+      </c>
+      <c r="L2">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18388CDF-BD22-4B44-B284-638AB54AAAF6}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -1234,11 +1371,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9FEB4D-EC75-4F1A-9E57-6A856A099F59}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -2127,7 +2264,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2259,8 +2396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD6177A-7BF6-452C-B399-7E27930614E1}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>